<commit_message>
me falta subirlo al servidor de la universidad
</commit_message>
<xml_diff>
--- a/programas.xlsx
+++ b/programas.xlsx
@@ -962,8 +962,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EACBC2B-383A-4AD3-9895-C826529D8501}">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:D185"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D182" sqref="D182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
arregle los progrmas que no aparecion, escuela de ingenieria
</commit_message>
<xml_diff>
--- a/programas.xlsx
+++ b/programas.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uredu-my.sharepoint.com/personal/luisfe_moreno_urosario_edu_co/Documents/calendario academico 2020 nuevo diseño/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="8_{B473892C-5A2C-40E3-95E7-760E73411A2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{554098B7-2BC2-489E-B20E-5AB844F69454}"/>
+  <xr:revisionPtr revIDLastSave="6" documentId="8_{B473892C-5A2C-40E3-95E7-760E73411A2C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{9EC66187-55DC-4F8C-A86C-5A172358FF68}"/>
   <bookViews>
     <workbookView xWindow="21480" yWindow="-120" windowWidth="20640" windowHeight="11160" xr2:uid="{73AB0902-A688-481F-BE1C-B5C376663794}"/>
   </bookViews>
   <sheets>
     <sheet name="programas" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">programas!$A$1:$D$185</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -962,8 +965,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EACBC2B-383A-4AD3-9895-C826529D8501}">
   <dimension ref="A1:D185"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="D182" sqref="D182"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18:B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>